<commit_message>
Details of requests for household recycling
</commit_message>
<xml_diff>
--- a/DCD_DataSheet.xlsx
+++ b/DCD_DataSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\odawkins\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\odawkins\Dropbox\Building_City_Dashboards\Data Coordination Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BD42F0-6C71-4E5A-9232-31488DE27395}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A94753A-2F79-4CB7-B6F2-441709D83B68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{523D2D9A-F482-4483-835D-05E2CE6BC87A}"/>
   </bookViews>
@@ -300,13 +300,13 @@
     <t>To be investigated</t>
   </si>
   <si>
-    <t>Update Request to be investigated</t>
-  </si>
-  <si>
     <t>Data Update Request</t>
   </si>
   <si>
-    <t>Data appears to have been scraped from National Waste Reports which stopped in 2012. Last official update was in Bulletin 2 report for 2013 (published 2014). 24/06/2019 - EPA are working on 2014 to 2016 data before sharing. Figures for 2017 will be available later in the year (www.wastereport.ie).</t>
+    <t>24/06/2019 - EPA are working on 2014 to 2016 data before sharing. Figures for 2017 will be available later in the year (www.wastereport.ie). Data appears to have been scraped from National Waste Reports which stopped in 2012. Last official update was in Bulletin 2 report for 2013 (published 2014).</t>
+  </si>
+  <si>
+    <t>24/06/2019 - Request for data added to enquiry on data for Waste per Capita (above)</t>
   </si>
 </sst>
 </file>
@@ -806,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438EDA1E-722D-41DF-AD57-5757E3B171A1}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -850,7 +850,7 @@
         <v>85</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>87</v>
@@ -882,7 +882,7 @@
         <v>43633</v>
       </c>
       <c r="I3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -911,7 +911,7 @@
         <v>43633</v>
       </c>
       <c r="I4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -940,7 +940,7 @@
         <v>43633</v>
       </c>
       <c r="I5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update housing data entry for DCD_Datasheet
</commit_message>
<xml_diff>
--- a/DCD_DataSheet.xlsx
+++ b/DCD_DataSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\odawkins\Dropbox\Building_City_Dashboards\Data Coordination Requests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam\Documents\repos\bcd-dd-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A94753A-2F79-4CB7-B6F2-441709D83B68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5197E6BC-3F26-406E-A8BC-5AF04EE6B1EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{523D2D9A-F482-4483-835D-05E2CE6BC87A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="93">
   <si>
     <t>Chart No</t>
   </si>
@@ -307,12 +307,15 @@
   </si>
   <si>
     <t>24/06/2019 - Request for data added to enquiry on data for Waste per Capita (above)</t>
+  </si>
+  <si>
+    <t>15/07/2019 - Data.gov and CSO mot recent dates 02/18 (LOS)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -455,7 +458,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -482,6 +485,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
@@ -494,8 +498,36 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{357E3DD9-237E-483E-9BE3-D470A78D0B2A}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -806,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438EDA1E-722D-41DF-AD57-5757E3B171A1}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,6 +1209,9 @@
       </c>
       <c r="G16" t="s">
         <v>33</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Data Sources in Table
</commit_message>
<xml_diff>
--- a/DCD_DataSheet.xlsx
+++ b/DCD_DataSheet.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam\Documents\repos\bcd-dd-v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5197E6BC-3F26-406E-A8BC-5AF04EE6B1EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{523D2D9A-F482-4483-835D-05E2CE6BC87A}"/>
+    <workbookView xWindow="40" yWindow="660" windowWidth="32180" windowHeight="18940"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Landing Page" sheetId="2" r:id="rId1"/>
+    <sheet name="Themes Page" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
   <si>
     <t>Chart No</t>
   </si>
@@ -310,13 +316,89 @@
   </si>
   <si>
     <t>15/07/2019 - Data.gov and CSO mot recent dates 02/18 (LOS)</t>
+  </si>
+  <si>
+    <t>Annual Population</t>
+  </si>
+  <si>
+    <t>Unemployment Quarterly Count</t>
+  </si>
+  <si>
+    <t>Monthly Property Price Index</t>
+  </si>
+  <si>
+    <t>Current most recent</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Full chart</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>/themes#population 
+'Population of Dublin'</t>
+  </si>
+  <si>
+    <t>/themes#employment 
+'Numbers Unemployed'</t>
+  </si>
+  <si>
+    <t>/themes#property-price-monthly 
+'Monthly Monthly Residential Property Price Index'</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/px/pxeirestat/Statire/SelectVarVal/Define.asp?maintable=HPM06&amp;PLanguage=0</t>
+  </si>
+  <si>
+    <t>Source file</t>
+  </si>
+  <si>
+    <t>https://www.cso.ie/px/pxeirestat/Statire/SelectVarVal/Define.asp?maintable=QLF08&amp;PLanguage=0</t>
+  </si>
+  <si>
+    <t>/themes#unitscompmonth
+Monthly House Unit Completions</t>
+  </si>
+  <si>
+    <t>2018Q3</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Verify Source Link</t>
+  </si>
+  <si>
+    <t>2019Q2</t>
+  </si>
+  <si>
+    <t>/data/Economy/QNQ22_2.csv</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Rename File</t>
+  </si>
+  <si>
+    <t>/data/Economy/QL408.csv</t>
+  </si>
+  <si>
+    <t>Source link is wrong</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,6 +459,21 @@
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -458,7 +555,7 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -486,6 +583,13 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
@@ -523,7 +627,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{357E3DD9-237E-483E-9BE3-D470A78D0B2A}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -835,31 +939,176 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438EDA1E-722D-41DF-AD57-5757E3B171A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A17:I22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+    <col min="3" max="3" width="53" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="36.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="59" customWidth="1"/>
-    <col min="3" max="3" width="51" customWidth="1"/>
+    <col min="3" max="3" width="81.83203125" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
+    <col min="6" max="6" width="35.1640625" customWidth="1"/>
+    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -888,7 +1137,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -917,7 +1166,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -946,7 +1195,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -975,7 +1224,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -1001,7 +1250,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -1027,7 +1276,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -1053,7 +1302,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -1079,12 +1328,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>1</v>
       </c>
@@ -1107,7 +1356,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>2</v>
       </c>
@@ -1130,7 +1379,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>3</v>
       </c>
@@ -1159,7 +1408,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>4</v>
       </c>
@@ -1188,7 +1437,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>5</v>
       </c>
@@ -1214,7 +1463,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>6</v>
       </c>
@@ -1243,7 +1492,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>7</v>
       </c>
@@ -1272,7 +1521,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>8</v>
       </c>
@@ -1295,7 +1544,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>9</v>
       </c>
@@ -1321,7 +1570,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>10</v>
       </c>
@@ -1347,12 +1596,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="21" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="11">
         <v>1</v>
       </c>
@@ -1378,7 +1627,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="11">
         <v>2</v>
       </c>
@@ -1398,7 +1647,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="11">
         <v>3</v>
       </c>
@@ -1418,7 +1667,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="11">
         <v>4</v>
       </c>
@@ -1440,25 +1689,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" location="demographics" display="http://localhost:3000/themes#demographics" xr:uid="{FB1E21EF-1A5E-4260-AFEF-A9623733D2F6}"/>
-    <hyperlink ref="C4" r:id="rId2" location=".VrNcerKLTIW" xr:uid="{15464721-73F7-482F-92CA-03F0FA53EB28}"/>
-    <hyperlink ref="C5" r:id="rId3" location=".VrNcerKLTIW" xr:uid="{75E22F02-C018-4814-86B4-51DB7F0025F7}"/>
-    <hyperlink ref="C8" r:id="rId4" xr:uid="{0DD168DE-FE8D-44CD-8015-66EEAE1227A4}"/>
-    <hyperlink ref="C12" r:id="rId5" xr:uid="{CB591FA0-0544-41E6-A0AF-8694F6C2EDBC}"/>
-    <hyperlink ref="C13" r:id="rId6" xr:uid="{6AEA3028-D30D-4F82-9F33-EBA4EFB12A37}"/>
-    <hyperlink ref="C14" r:id="rId7" xr:uid="{F66FE9E0-BFD0-4509-A8BE-7844534D5465}"/>
-    <hyperlink ref="C15" r:id="rId8" xr:uid="{A7F6E23E-2F66-4C7E-8B32-DD1F230A2CF7}"/>
-    <hyperlink ref="C16" r:id="rId9" xr:uid="{A3089E2D-4FD5-478F-81C9-E1D2DE927C63}"/>
-    <hyperlink ref="C17" r:id="rId10" xr:uid="{D23BDEA0-49D0-41B7-9E85-EAE076538AA0}"/>
-    <hyperlink ref="C18" r:id="rId11" xr:uid="{F6250F82-D80D-42EB-9061-F6BAAF4B10A2}"/>
-    <hyperlink ref="C20" r:id="rId12" xr:uid="{4D20D60B-A4F2-4577-BAE5-4BC384DF1D3B}"/>
-    <hyperlink ref="C21" r:id="rId13" xr:uid="{C0A2CD19-467A-4EB4-9FEE-81055173F263}"/>
-    <hyperlink ref="C22" r:id="rId14" xr:uid="{0EE337B1-1DB6-46AF-B2BC-9AD7C502EA98}"/>
-    <hyperlink ref="C24" r:id="rId15" xr:uid="{BBC710C4-7B5F-4197-AC40-48255C16CBE2}"/>
-    <hyperlink ref="C25" r:id="rId16" xr:uid="{C44F44A0-4A28-45FB-A1C4-21C7D602C663}"/>
-    <hyperlink ref="C26" r:id="rId17" xr:uid="{92968BD4-04C8-4BE3-96C9-BB883BA9EA6F}"/>
-    <hyperlink ref="C27" r:id="rId18" xr:uid="{9A1AEC3E-1BBB-4A7C-931F-DF0D9C04E702}"/>
-    <hyperlink ref="C3" r:id="rId19" location=".VrNcerKLTIW" xr:uid="{7F7B7437-EA4A-47BF-8FA7-BE79600DCCC8}"/>
+    <hyperlink ref="D3" r:id="rId1" location="demographics" display="http://localhost:3000/themes#demographics"/>
+    <hyperlink ref="C4" r:id="rId2" location=".VrNcerKLTIW"/>
+    <hyperlink ref="C5" r:id="rId3" location=".VrNcerKLTIW"/>
+    <hyperlink ref="C8" r:id="rId4"/>
+    <hyperlink ref="C12" r:id="rId5"/>
+    <hyperlink ref="C13" r:id="rId6"/>
+    <hyperlink ref="C14" r:id="rId7"/>
+    <hyperlink ref="C15" r:id="rId8"/>
+    <hyperlink ref="C16" r:id="rId9"/>
+    <hyperlink ref="C17" r:id="rId10"/>
+    <hyperlink ref="C18" r:id="rId11"/>
+    <hyperlink ref="C20" r:id="rId12"/>
+    <hyperlink ref="C21" r:id="rId13"/>
+    <hyperlink ref="C22" r:id="rId14"/>
+    <hyperlink ref="C24" r:id="rId15"/>
+    <hyperlink ref="C25" r:id="rId16"/>
+    <hyperlink ref="C26" r:id="rId17"/>
+    <hyperlink ref="C27" r:id="rId18"/>
+    <hyperlink ref="C3" r:id="rId19" location=".VrNcerKLTIW"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>

</xml_diff>

<commit_message>
Add data for quarterly hosuing completions#183, plot bars
</commit_message>
<xml_diff>
--- a/DCD_DataSheet.xlsx
+++ b/DCD_DataSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Documents/repos/bcd-dd-v2.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="880" windowWidth="32180" windowHeight="18940"/>
+    <workbookView minimized="1" xWindow="1560" yWindow="700" windowWidth="32180" windowHeight="18940"/>
   </bookViews>
   <sheets>
     <sheet name="Landing Page" sheetId="2" r:id="rId1"/>

</xml_diff>